<commit_message>
Moved new harcoded dialogue into the spreadsheet
</commit_message>
<xml_diff>
--- a/app/src/main/resources/spreadsheets/dialogue.xlsx
+++ b/app/src/main/resources/spreadsheets/dialogue.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/devel/ShootingStars/src/main/resources/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/Documents/devel/java/shooting-stars/app/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A0962B-A061-0945-9200-9541F1FD14DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96450CA-C00A-B148-B726-C2C92D8A02E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>DIALOGUE</t>
   </si>
@@ -213,6 +213,51 @@
   </si>
   <si>
     <t>Stiskněte klávesu “S” pro spuštění</t>
+  </si>
+  <si>
+    <t>deleteDataButton</t>
+  </si>
+  <si>
+    <t>Delete Data</t>
+  </si>
+  <si>
+    <t>My Instagram</t>
+  </si>
+  <si>
+    <t>Project GitHub</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>Smazat Data</t>
+  </si>
+  <si>
+    <t>데이터 삭제</t>
+  </si>
+  <si>
+    <t>データ削除</t>
+  </si>
+  <si>
+    <t>내 인스타그램</t>
+  </si>
+  <si>
+    <t>私のインスタグラム</t>
+  </si>
+  <si>
+    <t>Můj Instagram</t>
+  </si>
+  <si>
+    <t>프로젝트 깃허브</t>
+  </si>
+  <si>
+    <t>プロジェクト ギツハブ</t>
+  </si>
+  <si>
+    <t>GitHub Projektu</t>
   </si>
 </sst>
 </file>
@@ -635,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2AB3D20-1825-A34C-8076-B43BF1C24F7C}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -856,6 +901,57 @@
         <v>45</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fixed a typo in the korean start game dialogue
</commit_message>
<xml_diff>
--- a/app/src/main/resources/spreadsheets/dialogue.xlsx
+++ b/app/src/main/resources/spreadsheets/dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/Documents/devel/java/shooting-stars/app/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96450CA-C00A-B148-B726-C2C92D8A02E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41804EA-238E-6041-AE09-E9E196EA68F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
@@ -209,9 +209,6 @@
     <t>「S」キーを押してスタートしてください</t>
   </si>
   <si>
-    <t>‘R’ 키를 눌러 시작하세요</t>
-  </si>
-  <si>
     <t>Stiskněte klávesu “S” pro spuštění</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>GitHub Projektu</t>
+  </si>
+  <si>
+    <t>‘S’ 키를 눌러 시작하세요</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+      <selection pane="topRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -790,10 +790,10 @@
         <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
@@ -903,53 +903,53 @@
     </row>
     <row r="13" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed korean text font
</commit_message>
<xml_diff>
--- a/app/src/main/resources/spreadsheets/dialogue.xlsx
+++ b/app/src/main/resources/spreadsheets/dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejstastny/Documents/devel/java/shooting-stars/app/src/main/resources/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41804EA-238E-6041-AE09-E9E196EA68F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40BAFEB-1016-EE4B-9E63-673AB4C96210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{2BEE67CB-C7EF-534A-8A67-AA92EE8CA401}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>DIALOGUE</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>heading_KOR.ttf</t>
-  </si>
-  <si>
-    <t>defaultFont</t>
   </si>
   <si>
     <t>再起動するには 「R」 を押してください</t>
@@ -684,7 +681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D15" sqref="D15"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -742,7 +739,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>47</v>
@@ -787,16 +784,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,10 +875,10 @@
         <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
@@ -903,53 +900,53 @@
     </row>
     <row r="13" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>